<commit_message>
Update gh-pages to output generated at 14f1f32
</commit_message>
<xml_diff>
--- a/丽水-漫展信息.xlsx
+++ b/丽水-漫展信息.xlsx
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -521,7 +521,11 @@
       <c r="H2" t="b">
         <v>0</v>
       </c>
-      <c r="I2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=78294</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr">
         <is>
           <t>//i1.hdslb.com/bfs/openplatform/202311/lP5IkqWn1699431829470.jpeg</t>
@@ -553,7 +557,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -563,7 +567,11 @@
       <c r="H3" t="b">
         <v>0</v>
       </c>
-      <c r="I3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80714</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr">
         <is>
           <t>//i2.hdslb.com/bfs/openplatform/202401/rTvQio211704877379770.jpeg</t>
@@ -591,7 +599,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -601,7 +609,11 @@
       <c r="H4" t="b">
         <v>0</v>
       </c>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=81032</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr">
         <is>
           <t>//i0.hdslb.com/bfs/openplatform/202401/LbqTNkvq1705561884633.png</t>
@@ -633,7 +645,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -643,7 +655,11 @@
       <c r="H5" t="b">
         <v>0</v>
       </c>
-      <c r="I5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79437</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr">
         <is>
           <t>//i1.hdslb.com/bfs/openplatform/202312/ee5hLUN61702276208812.jpeg</t>
@@ -882,7 +898,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -892,7 +908,11 @@
       <c r="H2" t="b">
         <v>0</v>
       </c>
-      <c r="I2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=78294</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr">
         <is>
           <t>//i1.hdslb.com/bfs/openplatform/202311/lP5IkqWn1699431829470.jpeg</t>
@@ -924,7 +944,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -934,7 +954,11 @@
       <c r="H3" t="b">
         <v>0</v>
       </c>
-      <c r="I3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80714</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr">
         <is>
           <t>//i2.hdslb.com/bfs/openplatform/202401/rTvQio211704877379770.jpeg</t>
@@ -962,7 +986,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -972,7 +996,11 @@
       <c r="H4" t="b">
         <v>0</v>
       </c>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=81032</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr">
         <is>
           <t>//i0.hdslb.com/bfs/openplatform/202401/LbqTNkvq1705561884633.png</t>
@@ -1004,7 +1032,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -1014,7 +1042,11 @@
       <c r="H5" t="b">
         <v>0</v>
       </c>
-      <c r="I5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79437</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr">
         <is>
           <t>//i1.hdslb.com/bfs/openplatform/202312/ee5hLUN61702276208812.jpeg</t>

</xml_diff>

<commit_message>
Update gh-pages to output generated at 1f05065
</commit_message>
<xml_diff>
--- a/丽水-漫展信息.xlsx
+++ b/丽水-漫展信息.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,15 +472,10 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>是否有舞台（字符串匹配）</t>
+          <t>Link</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
         <is>
           <t>Cover</t>
         </is>
@@ -513,20 +508,15 @@
       <c r="F2" t="n">
         <v>289</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
+      <c r="G2" t="n">
+        <v>45</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=78294</t>
+        </is>
       </c>
       <c r="I2" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78294</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
         <is>
           <t>//i1.hdslb.com/bfs/openplatform/202311/lP5IkqWn1699431829470.jpeg</t>
         </is>
@@ -557,22 +547,17 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>226</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
+        <v>227</v>
+      </c>
+      <c r="G3" t="n">
+        <v>50</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80714</t>
+        </is>
       </c>
       <c r="I3" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80714</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
         <is>
           <t>//i2.hdslb.com/bfs/openplatform/202401/rTvQio211704877379770.jpeg</t>
         </is>
@@ -605,20 +590,15 @@
       <c r="F4" t="n">
         <v>32</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="H4" t="b">
-        <v>0</v>
+      <c r="G4" t="n">
+        <v>45</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=81032</t>
+        </is>
       </c>
       <c r="I4" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81032</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
         <is>
           <t>//i0.hdslb.com/bfs/openplatform/202401/LbqTNkvq1705561884633.png</t>
         </is>
@@ -651,20 +631,15 @@
       <c r="F5" t="n">
         <v>268</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="H5" t="b">
-        <v>0</v>
+      <c r="G5" t="n">
+        <v>45</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79437</t>
+        </is>
       </c>
       <c r="I5" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79437</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
         <is>
           <t>//i1.hdslb.com/bfs/openplatform/202312/ee5hLUN61702276208812.jpeg</t>
         </is>
@@ -681,7 +656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -725,15 +700,10 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>是否有舞台（字符串匹配）</t>
+          <t>Link</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
         <is>
           <t>Cover</t>
         </is>
@@ -750,7 +720,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -794,15 +764,10 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>是否有舞台（字符串匹配）</t>
+          <t>Link</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
         <is>
           <t>Cover</t>
         </is>
@@ -819,7 +784,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -863,15 +828,10 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>是否有舞台（字符串匹配）</t>
+          <t>Link</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
         <is>
           <t>Cover</t>
         </is>
@@ -904,20 +864,15 @@
       <c r="F2" t="n">
         <v>289</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
+      <c r="G2" t="n">
+        <v>45</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=78294</t>
+        </is>
       </c>
       <c r="I2" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78294</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
         <is>
           <t>//i1.hdslb.com/bfs/openplatform/202311/lP5IkqWn1699431829470.jpeg</t>
         </is>
@@ -948,22 +903,17 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>226</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
+        <v>227</v>
+      </c>
+      <c r="G3" t="n">
+        <v>50</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80714</t>
+        </is>
       </c>
       <c r="I3" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80714</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
         <is>
           <t>//i2.hdslb.com/bfs/openplatform/202401/rTvQio211704877379770.jpeg</t>
         </is>
@@ -996,20 +946,15 @@
       <c r="F4" t="n">
         <v>32</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="H4" t="b">
-        <v>0</v>
+      <c r="G4" t="n">
+        <v>45</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=81032</t>
+        </is>
       </c>
       <c r="I4" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81032</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
         <is>
           <t>//i0.hdslb.com/bfs/openplatform/202401/LbqTNkvq1705561884633.png</t>
         </is>
@@ -1042,20 +987,15 @@
       <c r="F5" t="n">
         <v>268</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="H5" t="b">
-        <v>0</v>
+      <c r="G5" t="n">
+        <v>45</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79437</t>
+        </is>
       </c>
       <c r="I5" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79437</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
         <is>
           <t>//i1.hdslb.com/bfs/openplatform/202312/ee5hLUN61702276208812.jpeg</t>
         </is>

</xml_diff>